<commit_message>
init 3 @serbayacar change to loking lines in text
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -22,148 +22,191 @@
     <t>08-20-12</t>
   </si>
   <si>
-    <t>Concentration</t>
-  </si>
-  <si>
-    <t>0.5um:  23187</t>
-  </si>
-  <si>
-    <t>1.0um:   4888</t>
-  </si>
-  <si>
-    <t>2.5um:   1715</t>
-  </si>
-  <si>
-    <t>5.0um:    103</t>
-  </si>
-  <si>
-    <t>10 um:     46</t>
-  </si>
-  <si>
-    <t>AT:   12.4  RH:   37.5</t>
-  </si>
-  <si>
-    <t>DP:    0.254WB:    7.8</t>
+    <t xml:space="preserve">Concentration
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5um:  23187
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0um:   4888
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5um:   1715
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0um:    103
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 um:     46
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT:   12.4  RH:   37.5  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP:    0.254WB:    7.8  
+</t>
   </si>
   <si>
     <t>08-16-29</t>
   </si>
   <si>
-    <t>0.5um:  60194</t>
-  </si>
-  <si>
-    <t>1.0um:   8553</t>
-  </si>
-  <si>
-    <t>2.5um:   1565</t>
-  </si>
-  <si>
-    <t>5.0um:    146</t>
-  </si>
-  <si>
-    <t>10 um:     45</t>
-  </si>
-  <si>
-    <t>AT:    9.1  RH:   43.0</t>
-  </si>
-  <si>
-    <t>DP:   -1.250WB:    5.5</t>
+    <t xml:space="preserve">0.5um:  60194
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0um:   8553
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5um:   1565
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0um:    146
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 um:     45
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT:    9.1  RH:   43.0  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP:   -1.250WB:    5.5  
+</t>
   </si>
   <si>
     <t>08-25-43</t>
   </si>
   <si>
-    <t>0.5um:  12890</t>
-  </si>
-  <si>
-    <t>1.0um:   1344</t>
-  </si>
-  <si>
-    <t>2.5um:    160</t>
-  </si>
-  <si>
-    <t>5.0um:     61</t>
-  </si>
-  <si>
-    <t>10 um:     19</t>
-  </si>
-  <si>
-    <t>AT:    9.0  RH:   49.2</t>
-  </si>
-  <si>
-    <t>DP:    0.255WB:    5.8</t>
+    <t xml:space="preserve">0.5um:  12890
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0um:   1344
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5um:    160
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0um:     61
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 um:     19
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT:    9.0  RH:   49.2  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP:    0.255WB:    5.8  
+</t>
   </si>
   <si>
     <t>08-23-17</t>
   </si>
   <si>
-    <t>0.5um:  48877</t>
-  </si>
-  <si>
-    <t>1.0um:   8107</t>
-  </si>
-  <si>
-    <t>2.5um:   2918</t>
-  </si>
-  <si>
-    <t>5.0um:    228</t>
-  </si>
-  <si>
-    <t>10 um:     93</t>
-  </si>
-  <si>
-    <t>AT:    8.0  RH:   51.2</t>
-  </si>
-  <si>
-    <t>DP:    0.250WB:    5.1</t>
+    <t xml:space="preserve">0.5um:  48877
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0um:   8107
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5um:   2918
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0um:    228
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 um:     93
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT:    8.0  RH:   51.2  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP:    0.250WB:    5.1  
+</t>
   </si>
   <si>
     <t>08-13-02</t>
   </si>
   <si>
-    <t>0.5um:  93978</t>
-  </si>
-  <si>
-    <t>1.0um:  13343</t>
-  </si>
-  <si>
-    <t>2.5um:   2259</t>
-  </si>
-  <si>
-    <t>5.0um:    147</t>
-  </si>
-  <si>
-    <t>10 um:     26</t>
-  </si>
-  <si>
-    <t>AT:   11.1  RH:   39.1</t>
-  </si>
-  <si>
-    <t>DP:    0.247WB:    6.9</t>
+    <t xml:space="preserve">0.5um:  93978
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0um:  13343
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5um:   2259
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0um:    147
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 um:     26
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT:   11.1  RH:   39.1  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP:    0.247WB:    6.9  
+</t>
   </si>
   <si>
     <t>08-28-42</t>
   </si>
   <si>
-    <t>0.5um: 138871</t>
-  </si>
-  <si>
-    <t>1.0um:  20509</t>
-  </si>
-  <si>
-    <t>2.5um:   2790</t>
-  </si>
-  <si>
-    <t>5.0um:    263</t>
-  </si>
-  <si>
-    <t>10 um:     47</t>
-  </si>
-  <si>
-    <t>AT:    8.1  RH:   49.2</t>
-  </si>
-  <si>
-    <t>DP:    0.247WB:    5.1</t>
+    <t xml:space="preserve">0.5um: 138871
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0um:  20509
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5um:   2790
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0um:    263
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 um:     47
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT:    8.1  RH:   49.2  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP:    0.247WB:    5.1  
+</t>
   </si>
 </sst>
 </file>

</xml_diff>